<commit_message>
added questionnaire to pnc_visit
</commit_message>
<xml_diff>
--- a/config-gandaki/forms/app/pnc_visit.xlsx
+++ b/config-gandaki/forms/app/pnc_visit.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\space\repo\medic\configs\config-moh-nepal\master-direct-client-messaging\forms\app\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\config-gandaki-training\config-gandaki\forms\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E824FF7-E1AD-44B0-A89F-42BEA9181609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{42D2B52E-325C-E146-BD0A-5B8C20832215}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">survey!$A$1:$AMI$1</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,8 +39,43 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="D45" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>@lal@medic.org please go through all these translations and get them corrected.
+e.g.
+यौनि -&gt; योनी
+पानि -&gt; पानी
+बगीरहेको -&gt; बगिरहेको
+Government officials are usually strict about Nepali language. It can be embarrassing for us at the training program.
+cc @prajwol@medic.org
+_Assigned to lal@medic.org_
+	-Binod Adhikary
+cc @nitin@medic.org
+	-Binod Adhikary
+Thank you sir, corrected hai. Jaya hosh!!
+	-Lal Kunwar</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="140">
   <si>
     <t>type</t>
   </si>
@@ -233,9 +267,6 @@
     <t>note</t>
   </si>
   <si>
-    <t>visit_count_note</t>
-  </si>
-  <si>
     <t>yes</t>
   </si>
   <si>
@@ -360,51 +391,11 @@
     <t>pnc_visit</t>
   </si>
   <si>
-    <t>**This is PNC Visit No. ${current_visit_count}**</t>
-  </si>
-  <si>
     <t>pnc_visit_done</t>
-  </si>
-  <si>
-    <t>Has her ${current_visit_count} been completed?</t>
   </si>
   <si>
     <t xml:space="preserve">
 प्रसवोत्तर जाँच</t>
-  </si>
-  <si>
-    <r>
-      <t>**</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>यो ${current_visit_count_ne} पीएनसी  जाँच हो ।</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>**</t>
-    </r>
   </si>
   <si>
     <t>if(instance('contact-summary')/context/delivery_date != '', instance('contact-summary')/context/delivery_date, .)</t>
@@ -416,21 +407,127 @@
     <t>if(${days_since_delivery} &lt;= 1,1, if(${days_since_delivery} &lt;= 5,2,  if(${days_since_delivery}  &lt;=16,3,  if(${days_since_delivery} &lt;= 44,4,4))))</t>
   </si>
   <si>
-    <t xml:space="preserve">
-के उहाँको ${current_visit_count_ne} पीएनसी जाँच गरिएको छ?</t>
+    <t>today() - decimal-date-time(../delivery_date)</t>
   </si>
   <si>
-    <t>today() - decimal-date-time(../delivery_date)</t>
+    <t>pnc_visit_mother_status</t>
+  </si>
+  <si>
+    <t>उच्च ज्वरो आएको छ ?</t>
+  </si>
+  <si>
+    <t>danger_sign</t>
+  </si>
+  <si>
+    <t>Fever</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Excesive vaginal bleeding </t>
+  </si>
+  <si>
+    <t>Will the body be spasm?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Severe continuous headache or blurred vision </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Severe lower abdominal pain </t>
+  </si>
+  <si>
+    <t>Foul-smelling white discharge from the vagina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Redness of Calf or swollen or difficulty in breathing or chest pain </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Difficulty in micturition or leak urine </t>
+  </si>
+  <si>
+    <t>Do you have mood and emotional swings?</t>
+  </si>
+  <si>
+    <t>In women who have given birth by surgery, is bleeding at the site of surgery, very painful?</t>
+  </si>
+  <si>
+    <t>Give the necessary advice to the Delivery women/household head and refer them to the mentioning everything in a referral card.
+Tell the date of arrival to understand the health condition.</t>
+  </si>
+  <si>
+    <t>योनिबाट अत्यधिक रक्तस्राव छ ?</t>
+  </si>
+  <si>
+    <t>शरिर बाउँडिने छ ?</t>
+  </si>
+  <si>
+    <t>कडा / लगातार टाउको दुख्ने वा दृष्टि धमिलो छ ?</t>
+  </si>
+  <si>
+    <t>तल्लो पेट कडा दुख्ने / तारन्तार बान्ता भइरहेको छ ?</t>
+  </si>
+  <si>
+    <t>योनी बाट सेतो गन्ध आउने पानी बगिरहेको छ ?</t>
+  </si>
+  <si>
+    <t>पिंडुला रातो भएको वा सुन्निएको, श्वास फेर्न गाह्रो हुने वा छाती दुखी रहेको छ ?</t>
+  </si>
+  <si>
+    <t>पिसाब सजिलै फेर्न नसक्ने वा पिसाब चुहिने छ ?</t>
+  </si>
+  <si>
+    <t>मुड र भावनात्मक परिवर्तन /दोधार भइरहन्छ ?</t>
+  </si>
+  <si>
+    <t>शल्यक्रिया गरेर प्रसूति गराएका महिलामा शल्यक्रिया गरेको ठाउँमा रगत बगिरहेको, निकै कडा दुखिरहेको छ ?</t>
+  </si>
+  <si>
+    <t>सुत्केरी महिला/घरमुलीलाई तुरुन्त आवश्यक सल्लाह दिई प्रेषण रिपोर्टमा सबै कुरा उल्लेख गरी प्रेषण गर्नुहोस् । 
+स्वास्थ्य अवस्था बुझ्नका लागि आउने मिति भन्नुहोस् ।</t>
+  </si>
+  <si>
+    <t>vaginal_bleeding</t>
+  </si>
+  <si>
+    <t>blurred_vision</t>
+  </si>
+  <si>
+    <t>abdominal_pain</t>
+  </si>
+  <si>
+    <t>chest_pain</t>
+  </si>
+  <si>
+    <t>leak_urine</t>
+  </si>
+  <si>
+    <t>spasm</t>
+  </si>
+  <si>
+    <t>smelling_vagina</t>
+  </si>
+  <si>
+    <t>mood_swings</t>
+  </si>
+  <si>
+    <t>painful_surgery</t>
+  </si>
+  <si>
+    <t>health_advice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Does ${patient_name} have any danger signs? Ask and examine. </t>
+  </si>
+  <si>
+    <t>${patient_name} मा कुनै खतराका सङ्केतहरु छन् कि, सोध्नु /जाँच गर्नुहोस् ।</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\-mm\-yyyy\ hh\-mm\-ss"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -459,12 +556,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -502,8 +593,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="&quot;Nunito Sans&quot;"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -551,6 +659,12 @@
         <fgColor rgb="FFFFCC99"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor rgb="FFBCAED5"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -578,9 +692,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -604,36 +718,51 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Input" xfId="1" builtinId="20"/>
@@ -644,35 +773,6 @@
       <font>
         <color rgb="FF000000"/>
         <name val="Arial"/>
-        <charset val="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <charset val="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <charset val="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <charset val="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <charset val="1"/>
       </font>
     </dxf>
     <dxf>
@@ -703,154 +803,156 @@
       <font>
         <color rgb="FF000000"/>
         <name val="Arial"/>
-        <charset val="1"/>
       </font>
     </dxf>
     <dxf>
       <font>
         <color rgb="FF000000"/>
         <name val="Arial"/>
-        <charset val="1"/>
       </font>
     </dxf>
     <dxf>
       <font>
         <color rgb="FF000000"/>
         <name val="Arial"/>
-        <charset val="1"/>
       </font>
     </dxf>
     <dxf>
       <font>
         <color rgb="FF000000"/>
         <name val="Arial"/>
-        <charset val="1"/>
       </font>
     </dxf>
     <dxf>
       <font>
         <color rgb="FF000000"/>
         <name val="Arial"/>
-        <charset val="1"/>
       </font>
     </dxf>
     <dxf>
       <font>
         <color rgb="FF000000"/>
         <name val="Arial"/>
-        <charset val="1"/>
       </font>
     </dxf>
     <dxf>
       <font>
         <color rgb="FF000000"/>
         <name val="Arial"/>
-        <charset val="1"/>
       </font>
     </dxf>
     <dxf>
       <font>
         <color rgb="FF000000"/>
         <name val="Arial"/>
-        <charset val="1"/>
       </font>
     </dxf>
     <dxf>
       <font>
         <color rgb="FF000000"/>
         <name val="Arial"/>
-        <charset val="1"/>
       </font>
     </dxf>
     <dxf>
       <font>
         <color rgb="FF000000"/>
         <name val="Arial"/>
-        <charset val="1"/>
       </font>
     </dxf>
     <dxf>
       <font>
         <color rgb="FF000000"/>
         <name val="Arial"/>
-        <charset val="1"/>
       </font>
     </dxf>
     <dxf>
       <font>
         <color rgb="FF000000"/>
         <name val="Arial"/>
-        <charset val="1"/>
       </font>
     </dxf>
     <dxf>
       <font>
         <color rgb="FF000000"/>
         <name val="Arial"/>
-        <charset val="1"/>
       </font>
     </dxf>
     <dxf>
       <font>
         <color rgb="FF000000"/>
         <name val="Arial"/>
-        <charset val="1"/>
       </font>
     </dxf>
     <dxf>
       <font>
         <color rgb="FF000000"/>
         <name val="Arial"/>
-        <charset val="1"/>
       </font>
     </dxf>
     <dxf>
       <font>
         <color rgb="FF000000"/>
         <name val="Arial"/>
-        <charset val="1"/>
       </font>
     </dxf>
     <dxf>
       <font>
         <color rgb="FF000000"/>
         <name val="Arial"/>
-        <charset val="1"/>
       </font>
     </dxf>
     <dxf>
       <font>
         <color rgb="FF000000"/>
         <name val="Arial"/>
-        <charset val="1"/>
       </font>
     </dxf>
     <dxf>
       <font>
         <color rgb="FF000000"/>
         <name val="Arial"/>
-        <charset val="1"/>
       </font>
     </dxf>
     <dxf>
       <font>
         <color rgb="FF000000"/>
         <name val="Arial"/>
-        <charset val="1"/>
       </font>
     </dxf>
     <dxf>
       <font>
         <color rgb="FF000000"/>
         <name val="Arial"/>
-        <charset val="1"/>
       </font>
     </dxf>
     <dxf>
       <font>
         <color rgb="FF000000"/>
         <name val="Arial"/>
-        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
       </font>
     </dxf>
   </dxfs>
@@ -1162,35 +1264,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A35A47E4-BCDA-F641-B88C-C95981BF88E3}">
-  <dimension ref="A1:AMJ40"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AMJ51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C23" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="102" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="19.8984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.59765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.8984375" customWidth="1"/>
-    <col min="4" max="4" width="46.19921875" customWidth="1"/>
-    <col min="5" max="5" width="11.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.875" customWidth="1"/>
+    <col min="4" max="4" width="46.25" customWidth="1"/>
+    <col min="5" max="5" width="11.375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4.5" customWidth="1"/>
-    <col min="7" max="7" width="13.8984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.59765625" customWidth="1"/>
-    <col min="10" max="10" width="4.8984375" customWidth="1"/>
-    <col min="11" max="11" width="40.69921875" customWidth="1"/>
-    <col min="12" max="12" width="13.8984375" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="10.3984375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.8984375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.09765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.625" customWidth="1"/>
+    <col min="10" max="10" width="4.875" customWidth="1"/>
+    <col min="11" max="11" width="40.75" customWidth="1"/>
+    <col min="12" max="12" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.8984375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1023" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1023" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2251,7 +2353,7 @@
       <c r="AMH1" s="4"/>
       <c r="AMI1" s="4"/>
     </row>
-    <row r="2" spans="1:1023" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1023" ht="15.75" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>18</v>
       </c>
@@ -3288,7 +3390,7 @@
       <c r="AMH2" s="4"/>
       <c r="AMI2" s="4"/>
     </row>
-    <row r="3" spans="1:1023" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1023" ht="14.45" customHeight="1">
       <c r="A3" s="5" t="s">
         <v>24</v>
       </c>
@@ -4323,7 +4425,7 @@
       <c r="AMH3" s="4"/>
       <c r="AMI3" s="4"/>
     </row>
-    <row r="4" spans="1:1023" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1023" ht="15.75" customHeight="1">
       <c r="A4" s="5" t="s">
         <v>24</v>
       </c>
@@ -5356,7 +5458,7 @@
       <c r="AMH4" s="4"/>
       <c r="AMI4" s="4"/>
     </row>
-    <row r="5" spans="1:1023" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1023" ht="15.75" customHeight="1">
       <c r="A5" s="5" t="s">
         <v>18</v>
       </c>
@@ -6389,7 +6491,7 @@
       <c r="AMH5" s="4"/>
       <c r="AMI5" s="4"/>
     </row>
-    <row r="6" spans="1:1023" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1023" ht="15.75" customHeight="1">
       <c r="A6" s="5" t="s">
         <v>32</v>
       </c>
@@ -7424,7 +7526,7 @@
       <c r="AMH6" s="4"/>
       <c r="AMI6" s="4"/>
     </row>
-    <row r="7" spans="1:1023" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1023" ht="15.75" customHeight="1">
       <c r="A7" s="5" t="s">
         <v>24</v>
       </c>
@@ -8457,7 +8559,7 @@
       <c r="AMH7" s="4"/>
       <c r="AMI7" s="4"/>
     </row>
-    <row r="8" spans="1:1023" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1023" ht="15.75" customHeight="1">
       <c r="A8" s="5" t="s">
         <v>24</v>
       </c>
@@ -9490,7 +9592,7 @@
       <c r="AMH8" s="4"/>
       <c r="AMI8" s="4"/>
     </row>
-    <row r="9" spans="1:1023" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1023" ht="15.75" customHeight="1">
       <c r="A9" s="5" t="s">
         <v>24</v>
       </c>
@@ -10525,7 +10627,7 @@
       <c r="AMH9" s="4"/>
       <c r="AMI9" s="4"/>
     </row>
-    <row r="10" spans="1:1023" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1023" ht="15.75" customHeight="1">
       <c r="A10" s="5" t="s">
         <v>24</v>
       </c>
@@ -11558,7 +11660,7 @@
       <c r="AMH10" s="4"/>
       <c r="AMI10" s="4"/>
     </row>
-    <row r="11" spans="1:1023" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1023" ht="15.75" customHeight="1">
       <c r="A11" s="5" t="s">
         <v>18</v>
       </c>
@@ -12591,7 +12693,7 @@
       <c r="AMH11" s="4"/>
       <c r="AMI11" s="4"/>
     </row>
-    <row r="12" spans="1:1023" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1023" ht="15.75" customHeight="1">
       <c r="A12" s="5" t="s">
         <v>24</v>
       </c>
@@ -13624,7 +13726,7 @@
       <c r="AMH12" s="4"/>
       <c r="AMI12" s="4"/>
     </row>
-    <row r="13" spans="1:1023" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1023" ht="15.75" customHeight="1">
       <c r="A13" s="5" t="s">
         <v>18</v>
       </c>
@@ -14657,7 +14759,7 @@
       <c r="AMH13" s="4"/>
       <c r="AMI13" s="4"/>
     </row>
-    <row r="14" spans="1:1023" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1023" ht="15.75" customHeight="1">
       <c r="A14" s="5" t="s">
         <v>24</v>
       </c>
@@ -15690,7 +15792,7 @@
       <c r="AMH14" s="4"/>
       <c r="AMI14" s="4"/>
     </row>
-    <row r="15" spans="1:1023" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1023" ht="15.75" customHeight="1">
       <c r="A15" s="5" t="s">
         <v>18</v>
       </c>
@@ -16723,7 +16825,7 @@
       <c r="AMH15" s="4"/>
       <c r="AMI15" s="4"/>
     </row>
-    <row r="16" spans="1:1023" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1023" ht="15.75" customHeight="1">
       <c r="A16" s="5" t="s">
         <v>24</v>
       </c>
@@ -17756,7 +17858,7 @@
       <c r="AMH16" s="4"/>
       <c r="AMI16" s="4"/>
     </row>
-    <row r="17" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1024" ht="15.75" customHeight="1">
       <c r="A17" s="5" t="s">
         <v>24</v>
       </c>
@@ -18789,7 +18891,7 @@
       <c r="AMH17" s="4"/>
       <c r="AMI17" s="4"/>
     </row>
-    <row r="18" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1024" ht="15.75" customHeight="1">
       <c r="A18" s="5" t="s">
         <v>52</v>
       </c>
@@ -19818,7 +19920,7 @@
       <c r="AMH18" s="4"/>
       <c r="AMI18" s="4"/>
     </row>
-    <row r="19" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1024" ht="15.75" customHeight="1">
       <c r="A19" s="5" t="s">
         <v>52</v>
       </c>
@@ -20847,7 +20949,7 @@
       <c r="AMH19" s="4"/>
       <c r="AMI19" s="4"/>
     </row>
-    <row r="20" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1024" ht="15.75" customHeight="1">
       <c r="A20" s="5" t="s">
         <v>52</v>
       </c>
@@ -21876,7 +21978,7 @@
       <c r="AMH20" s="4"/>
       <c r="AMI20" s="4"/>
     </row>
-    <row r="21" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1024" ht="15.75" customHeight="1">
       <c r="A21" s="5" t="s">
         <v>52</v>
       </c>
@@ -22905,7 +23007,7 @@
       <c r="AMH21" s="4"/>
       <c r="AMI21" s="4"/>
     </row>
-    <row r="22" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1024" ht="15.75" customHeight="1">
       <c r="A22" s="5" t="s">
         <v>52</v>
       </c>
@@ -23934,12 +24036,12 @@
       <c r="AMH22" s="4"/>
       <c r="AMI22" s="4"/>
     </row>
-    <row r="23" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="23" t="s">
+    <row r="23" spans="1:1024" ht="15.75" customHeight="1">
+      <c r="A23" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="B23" s="23" t="s">
-        <v>82</v>
+      <c r="B23" s="22" t="s">
+        <v>81</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>21</v>
@@ -23954,7 +24056,7 @@
       <c r="I23" s="6"/>
       <c r="J23" s="6"/>
       <c r="K23" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L23" s="6"/>
       <c r="M23" s="6"/>
@@ -24970,12 +25072,12 @@
       <c r="AMI23" s="4"/>
       <c r="AMJ23" s="4"/>
     </row>
-    <row r="24" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="23" t="s">
+    <row r="24" spans="1:1024" ht="15.75" customHeight="1">
+      <c r="A24" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="B24" s="23" t="s">
-        <v>84</v>
+      <c r="B24" s="22" t="s">
+        <v>83</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>21</v>
@@ -24990,7 +25092,7 @@
       <c r="I24" s="6"/>
       <c r="J24" s="6"/>
       <c r="K24" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L24" s="6"/>
       <c r="M24" s="6"/>
@@ -26008,11 +26110,11 @@
       <c r="AMI24" s="4"/>
       <c r="AMJ24" s="4"/>
     </row>
-    <row r="25" spans="1:1024" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="23" t="s">
+    <row r="25" spans="1:1024" ht="15.75" customHeight="1">
+      <c r="A25" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="B25" s="23" t="s">
+      <c r="B25" s="22" t="s">
         <v>38</v>
       </c>
       <c r="C25" s="6" t="s">
@@ -26022,7 +26124,7 @@
         <v>21</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
@@ -26030,7 +26132,7 @@
       <c r="I25" s="6"/>
       <c r="J25" s="6"/>
       <c r="K25" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L25" s="6"/>
       <c r="M25" s="6"/>
@@ -27048,12 +27150,12 @@
       <c r="AMI25" s="4"/>
       <c r="AMJ25" s="4"/>
     </row>
-    <row r="26" spans="1:1024" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="23" t="s">
+    <row r="26" spans="1:1024" ht="16.5" customHeight="1">
+      <c r="A26" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="B26" s="23" t="s">
-        <v>87</v>
+      <c r="B26" s="22" t="s">
+        <v>86</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>21</v>
@@ -27068,7 +27170,7 @@
       <c r="I26" s="7"/>
       <c r="J26" s="6"/>
       <c r="K26" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L26" s="7"/>
       <c r="M26" s="7"/>
@@ -28086,12 +28188,12 @@
       <c r="AMI26" s="4"/>
       <c r="AMJ26" s="4"/>
     </row>
-    <row r="27" spans="1:1024" x14ac:dyDescent="0.3">
-      <c r="A27" s="20" t="s">
+    <row r="27" spans="1:1024">
+      <c r="A27" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="B27" s="20" t="s">
-        <v>89</v>
+      <c r="B27" s="19" t="s">
+        <v>88</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>21</v>
@@ -28106,7 +28208,7 @@
       <c r="I27" s="7"/>
       <c r="J27" s="3"/>
       <c r="K27" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
@@ -29117,12 +29219,12 @@
       <c r="AMB27" s="3"/>
       <c r="AMC27" s="3"/>
     </row>
-    <row r="28" spans="1:1024" x14ac:dyDescent="0.3">
-      <c r="A28" s="20" t="s">
+    <row r="28" spans="1:1024">
+      <c r="A28" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="B28" s="20" t="s">
-        <v>96</v>
+      <c r="B28" s="19" t="s">
+        <v>95</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>21</v>
@@ -29137,7 +29239,7 @@
       <c r="I28" s="7"/>
       <c r="J28" s="3"/>
       <c r="K28" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L28" s="3"/>
       <c r="M28" s="3"/>
@@ -30148,12 +30250,12 @@
       <c r="AMB28" s="3"/>
       <c r="AMC28" s="3"/>
     </row>
-    <row r="29" spans="1:1024" x14ac:dyDescent="0.3">
-      <c r="A29" s="20" t="s">
+    <row r="29" spans="1:1024">
+      <c r="A29" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="B29" s="20" t="s">
-        <v>97</v>
+      <c r="B29" s="19" t="s">
+        <v>96</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>21</v>
@@ -30167,8 +30269,8 @@
       <c r="H29" s="3"/>
       <c r="I29" s="7"/>
       <c r="J29" s="3"/>
-      <c r="K29" s="24" t="s">
-        <v>95</v>
+      <c r="K29" s="23" t="s">
+        <v>94</v>
       </c>
       <c r="L29" s="3"/>
       <c r="M29" s="3"/>
@@ -31177,12 +31279,12 @@
       <c r="AMB29" s="3"/>
       <c r="AMC29" s="3"/>
     </row>
-    <row r="30" spans="1:1024" x14ac:dyDescent="0.3">
-      <c r="A30" s="20" t="s">
+    <row r="30" spans="1:1024">
+      <c r="A30" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="B30" s="20" t="s">
-        <v>92</v>
+      <c r="B30" s="19" t="s">
+        <v>91</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>21</v>
@@ -31197,7 +31299,7 @@
       <c r="I30" s="7"/>
       <c r="J30" s="3"/>
       <c r="K30" s="3" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="L30" s="3"/>
       <c r="M30" s="3"/>
@@ -32208,12 +32310,12 @@
       <c r="AMB30" s="3"/>
       <c r="AMC30" s="3"/>
     </row>
-    <row r="31" spans="1:1024" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="A31" s="20" t="s">
+    <row r="31" spans="1:1024" ht="57">
+      <c r="A31" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="B31" s="20" t="s">
-        <v>76</v>
+      <c r="B31" s="19" t="s">
+        <v>75</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>21</v>
@@ -32227,8 +32329,8 @@
       <c r="H31" s="3"/>
       <c r="I31" s="7"/>
       <c r="J31" s="3"/>
-      <c r="K31" s="22" t="s">
-        <v>106</v>
+      <c r="K31" s="21" t="s">
+        <v>102</v>
       </c>
       <c r="L31" s="3"/>
       <c r="M31" s="3"/>
@@ -33239,12 +33341,12 @@
       <c r="AMB31" s="3"/>
       <c r="AMC31" s="3"/>
     </row>
-    <row r="32" spans="1:1024" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="A32" s="20" t="s">
+    <row r="32" spans="1:1024" ht="57">
+      <c r="A32" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="B32" s="20" t="s">
-        <v>77</v>
+      <c r="B32" s="19" t="s">
+        <v>76</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>21</v>
@@ -33258,8 +33360,8 @@
       <c r="H32" s="3"/>
       <c r="I32" s="7"/>
       <c r="J32" s="3"/>
-      <c r="K32" s="22" t="s">
-        <v>91</v>
+      <c r="K32" s="21" t="s">
+        <v>90</v>
       </c>
       <c r="L32" s="3"/>
       <c r="M32" s="3"/>
@@ -34268,7 +34370,7 @@
       <c r="AMB32" s="3"/>
       <c r="AMC32" s="3"/>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:22">
       <c r="A33" s="10" t="s">
         <v>18</v>
       </c>
@@ -34302,12 +34404,12 @@
       <c r="U33" s="3"/>
       <c r="V33" s="3"/>
     </row>
-    <row r="34" spans="1:22" ht="55.8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:22" ht="57.75">
       <c r="A34" s="10" t="s">
         <v>54</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>21</v>
@@ -34322,7 +34424,7 @@
       <c r="I34" s="7"/>
       <c r="J34" s="3"/>
       <c r="K34" s="7" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="L34" s="3"/>
       <c r="M34" s="3"/>
@@ -34338,7 +34440,7 @@
       <c r="U34" s="3"/>
       <c r="V34" s="3"/>
     </row>
-    <row r="35" spans="1:22" ht="28.2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:22" ht="29.25">
       <c r="A35" s="10" t="s">
         <v>54</v>
       </c>
@@ -34358,7 +34460,7 @@
       <c r="I35" s="7"/>
       <c r="J35" s="3"/>
       <c r="K35" s="7" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="L35" s="3"/>
       <c r="M35" s="3"/>
@@ -34374,7 +34476,7 @@
       <c r="U35" s="3"/>
       <c r="V35" s="3"/>
     </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:22">
       <c r="A36" s="10" t="s">
         <v>52</v>
       </c>
@@ -34382,102 +34484,249 @@
         <v>53</v>
       </c>
     </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A37" s="11" t="s">
+    <row r="37" spans="1:22" s="25" customFormat="1">
+      <c r="A37" s="24"/>
+      <c r="B37" s="24"/>
+      <c r="Q37" s="24"/>
+    </row>
+    <row r="38" spans="1:22" s="28" customFormat="1">
+      <c r="A38" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="B37" s="11" t="s">
-        <v>98</v>
+      <c r="B38" s="26" t="s">
+        <v>104</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C38" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="D38" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="G37" t="s">
+      <c r="G38" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="Q37" s="3" t="s">
+      <c r="Q38" s="27" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A38" s="11" t="s">
+    <row r="39" spans="1:22" s="28" customFormat="1" ht="25.5">
+      <c r="A39" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="B39" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="C39" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="D39" s="31" t="s">
+        <v>139</v>
+      </c>
+      <c r="E39" s="27"/>
+      <c r="F39" s="27"/>
+      <c r="G39" s="27"/>
+      <c r="H39" s="27"/>
+      <c r="I39" s="29"/>
+      <c r="J39" s="27"/>
+      <c r="K39" s="27"/>
+      <c r="L39" s="27"/>
+      <c r="M39" s="27"/>
+      <c r="N39" s="27"/>
+      <c r="O39" s="27"/>
+      <c r="P39" s="27"/>
+      <c r="Q39" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="R39" s="27"/>
+      <c r="S39" s="27"/>
+      <c r="T39" s="27"/>
+      <c r="U39" s="27"/>
+      <c r="V39" s="27"/>
+    </row>
+    <row r="40" spans="1:22" s="28" customFormat="1">
+      <c r="A40" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="B40" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="C40" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="D40" s="31" t="s">
+        <v>105</v>
+      </c>
+      <c r="E40" s="27"/>
+      <c r="F40" s="27"/>
+      <c r="G40" s="27"/>
+      <c r="H40" s="27"/>
+      <c r="I40" s="29"/>
+      <c r="J40" s="27"/>
+      <c r="K40" s="27"/>
+      <c r="L40" s="27"/>
+      <c r="M40" s="27"/>
+      <c r="N40" s="27"/>
+      <c r="O40" s="27"/>
+      <c r="P40" s="27"/>
+      <c r="Q40" s="27"/>
+      <c r="R40" s="27"/>
+      <c r="S40" s="27"/>
+      <c r="T40" s="27"/>
+      <c r="U40" s="27"/>
+      <c r="V40" s="27"/>
+    </row>
+    <row r="41" spans="1:22" s="28" customFormat="1">
+      <c r="A41" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="B41" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="C41" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="D41" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q41" s="27" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22" s="28" customFormat="1">
+      <c r="A42" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="B42" s="26" t="s">
+        <v>133</v>
+      </c>
+      <c r="C42" s="31" t="s">
+        <v>109</v>
+      </c>
+      <c r="D42" s="31" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22" s="28" customFormat="1">
+      <c r="A43" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="B43" s="26" t="s">
+        <v>129</v>
+      </c>
+      <c r="C43" s="31" t="s">
+        <v>110</v>
+      </c>
+      <c r="D43" s="31" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22" s="28" customFormat="1">
+      <c r="A44" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="B44" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="C44" s="32" t="s">
+        <v>111</v>
+      </c>
+      <c r="D44" s="31" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22" s="28" customFormat="1">
+      <c r="A45" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="B45" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="C45" s="31" t="s">
+        <v>112</v>
+      </c>
+      <c r="D45" s="31" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22" s="28" customFormat="1" ht="25.5">
+      <c r="A46" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="B46" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="C46" s="31" t="s">
+        <v>113</v>
+      </c>
+      <c r="D46" s="33" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22" s="28" customFormat="1">
+      <c r="A47" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="B47" s="26" t="s">
+        <v>132</v>
+      </c>
+      <c r="C47" s="31" t="s">
+        <v>114</v>
+      </c>
+      <c r="D47" s="31" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="48" spans="1:22" s="28" customFormat="1">
+      <c r="A48" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="B48" s="26" t="s">
+        <v>135</v>
+      </c>
+      <c r="C48" s="31" t="s">
+        <v>115</v>
+      </c>
+      <c r="D48" s="31" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" s="28" customFormat="1" ht="25.5">
+      <c r="A49" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="B49" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="C49" s="31" t="s">
+        <v>116</v>
+      </c>
+      <c r="D49" s="31" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" s="28" customFormat="1" ht="76.5">
+      <c r="A50" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="B38" s="11" t="s">
-        <v>57</v>
+      <c r="B50" s="26" t="s">
+        <v>137</v>
       </c>
-      <c r="C38" s="7" t="s">
-        <v>99</v>
+      <c r="C50" s="31" t="s">
+        <v>117</v>
       </c>
-      <c r="D38" s="3" t="s">
-        <v>103</v>
+      <c r="D50" s="31" t="s">
+        <v>127</v>
       </c>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
-      <c r="H38" s="3"/>
-      <c r="I38" s="7"/>
-      <c r="J38" s="3"/>
-      <c r="K38" s="3"/>
-      <c r="L38" s="3"/>
-      <c r="M38" s="3"/>
-      <c r="N38" s="3"/>
-      <c r="O38" s="3"/>
-      <c r="P38" s="3"/>
-      <c r="Q38" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="R38" s="3"/>
-      <c r="S38" s="3"/>
-      <c r="T38" s="3"/>
-      <c r="U38" s="3"/>
-      <c r="V38" s="3"/>
     </row>
-    <row r="39" spans="1:22" ht="28.2" x14ac:dyDescent="0.3">
-      <c r="A39" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="B39" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="D39" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
-      <c r="I39" s="7"/>
-      <c r="J39" s="3"/>
-      <c r="K39" s="3"/>
-      <c r="L39" s="3"/>
-      <c r="M39" s="3"/>
-      <c r="N39" s="3"/>
-      <c r="O39" s="3"/>
-      <c r="P39" s="3"/>
-      <c r="Q39" s="3"/>
-      <c r="R39" s="3"/>
-      <c r="S39" s="3"/>
-      <c r="T39" s="3"/>
-      <c r="U39" s="3"/>
-      <c r="V39" s="3"/>
-    </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A40" s="11" t="s">
+    <row r="51" spans="1:4" s="28" customFormat="1">
+      <c r="A51" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="B40" s="11" t="s">
-        <v>98</v>
+      <c r="B51" s="35" t="s">
+        <v>104</v>
       </c>
-      <c r="Q40" s="3" t="s">
-        <v>24</v>
-      </c>
+      <c r="C51" s="34"/>
+      <c r="D51" s="34"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A26">
@@ -34511,7 +34760,7 @@
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B22">
     <cfRule type="expression" dxfId="23" priority="22">
-      <formula>COUNTIF($B$2:$B$107,#REF!)&gt;1</formula>
+      <formula>COUNTIF($B$2:$B$104,#REF!)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23">
@@ -34521,7 +34770,7 @@
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:B26">
     <cfRule type="expression" dxfId="21" priority="15">
-      <formula>COUNTIF($B$2:$B$94,#REF!)&gt;1</formula>
+      <formula>COUNTIF($B$2:$B$91,#REF!)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:C22">
@@ -34608,36 +34857,37 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" sqref="E2:E26" xr:uid="{259328CB-E096-4B9A-8CE0-E6E537CD0202}">
+    <dataValidation type="list" allowBlank="1" sqref="E2:E26">
       <formula1>"yes,no"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{065A0A7D-5130-954D-91D3-9CC87DBE51D7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
-        <v>59</v>
+    <row r="1" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A1" s="11" t="s">
+        <v>58</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="13" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="4"/>
@@ -34654,60 +34904,60 @@
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
     </row>
-    <row r="2" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="30">
       <c r="A2" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="D2" s="15" t="s">
+    </row>
+    <row r="3" spans="1:17">
+      <c r="A3" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>62</v>
       </c>
+      <c r="C3" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>64</v>
+      </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+    <row r="4" spans="1:17">
+      <c r="A4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" t="s">
         <v>60</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="D4" s="20" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="A5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>79</v>
-      </c>
-      <c r="B4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C4" t="s">
-        <v>61</v>
-      </c>
-      <c r="D4" s="21" t="s">
+      <c r="D5" s="20" t="s">
         <v>80</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>79</v>
-      </c>
-      <c r="B5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C5" t="s">
-        <v>64</v>
-      </c>
-      <c r="D5" s="21" t="s">
-        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -34716,61 +34966,61 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C260E274-4176-7E4D-9851-80893C793365}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="3" max="3" width="18.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="28.2" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:7" ht="30">
+      <c r="A1" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="E1" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="F1" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="G1" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="G1" s="16" t="s">
+    </row>
+    <row r="2" spans="1:7" ht="29.25">
+      <c r="A2" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="C2" s="17">
+        <f ca="1">NOW()</f>
+        <v>45769.655270833333</v>
+      </c>
+      <c r="D2" s="16" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="28.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
-        <v>102</v>
-      </c>
-      <c r="B2" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="C2" s="18">
-        <f ca="1">NOW()</f>
-        <v>45526.992813657409</v>
-      </c>
-      <c r="D2" s="17" t="s">
+      <c r="E2" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="F2" s="4"/>
+      <c r="G2" s="18" t="s">
         <v>74</v>
-      </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="19" t="s">
-        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>